<commit_message>
blank import and code improvement
</commit_message>
<xml_diff>
--- a/ExcelData/userLogin.xlsx
+++ b/ExcelData/userLogin.xlsx
@@ -32,10 +32,10 @@
     <t>Password</t>
   </si>
   <si>
-    <t>tarun_AM</t>
+    <t>admin@123</t>
   </si>
   <si>
-    <t>admin@123</t>
+    <t>visulonsprint</t>
   </si>
 </sst>
 </file>
@@ -376,7 +376,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -395,10 +395,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>